<commit_message>
[woo] actor data 오류 수정
</commit_message>
<xml_diff>
--- a/GameData/Excel/actor.xlsx
+++ b/GameData/Excel/actor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193A8F95-7967-4CCB-B009-64798CABF746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DBF6A-4F65-4F4D-B2E0-DB4CE18B07B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7968" yWindow="10368" windowWidth="34560" windowHeight="18792" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="4176" yWindow="14160" windowWidth="15060" windowHeight="11436" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="actor" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4:E5"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
@@ -645,7 +645,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2000001</v>
+        <v>20001</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>

</xml_diff>